<commit_message>
fix typo and update experiment_plan
</commit_message>
<xml_diff>
--- a/report/experiment_plan.xlsx
+++ b/report/experiment_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengchen/GitHub/master_thesis/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3051466F-F8DE-984E-9DBF-94AF48A66761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2828E61-B4FC-AF45-9EF1-3E215248412F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
   </bookViews>
   <sheets>
     <sheet name="plan_50_trials" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="33">
   <si>
     <t>ACQ function</t>
   </si>
@@ -91,9 +91,6 @@
     <t>Remark</t>
   </si>
   <si>
-    <t>Benchmark</t>
-  </si>
-  <si>
     <t>✅</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>EI</t>
   </si>
   <si>
-    <t>explore the impact of acquisition function</t>
-  </si>
-  <si>
     <t>random_sampling</t>
   </si>
   <si>
@@ -125,6 +119,24 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>explore the impact of acquisition function (train_test_split=0.5, num_init=10)</t>
+  </si>
+  <si>
+    <t>explore_factor=0.75. Rationale: left skewed; if set to too high value, extreme quantiles have less observation and might have less reliable estimation.</t>
+  </si>
+  <si>
+    <t>optimum: 91.57</t>
+  </si>
+  <si>
+    <t>optimum: 73.25999</t>
+  </si>
+  <si>
+    <t>optimum: 47.33333</t>
   </si>
 </sst>
 </file>
@@ -148,15 +160,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -164,11 +188,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -186,10 +228,37 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +580,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L17" sqref="L17:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,13 +623,16 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>15</v>
@@ -569,7 +641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -592,19 +664,23 @@
         <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="11">
+        <v>91.148399999999995</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.28520000000000001</v>
+      </c>
+      <c r="K2" s="3">
+        <f>J2/I2</f>
+        <v>3.1289633169644233E-3</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3">
-        <v>91.148399999999995</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0.28510000000000002</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>17</v>
+      <c r="M2" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -612,7 +688,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -624,29 +700,33 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="3">
-        <v>72.691100000000006</v>
+        <v>91.058599999999998</v>
       </c>
       <c r="J3" s="3">
-        <v>0.62749999999999995</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
+        <v>0.3024</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K17" si="0">J3/I3</f>
+        <v>3.3209383847324692E-3</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="14"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -658,22 +738,26 @@
         <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.5</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3">
-        <v>46.804000000000002</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.43819999999999998</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="I4" s="12">
+        <v>91.130399999999995</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" si="0"/>
+        <v>2.5458024983979004E-3</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -689,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>7</v>
@@ -698,55 +782,65 @@
         <v>0.3</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="3">
-        <v>91.058599999999998</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.3024</v>
-      </c>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>91.113</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0.22520000000000001</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>2.4716560754228269E-3</v>
+      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="7">
         <v>0.5</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="3">
-        <v>91.130399999999995</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="L6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="7">
+        <v>91.040800000000004</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.2427</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6658377342905597E-3</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
@@ -755,31 +849,38 @@
         <v>2</v>
       </c>
       <c r="E7" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.3</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="3">
-        <v>91.113</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.22520000000000001</v>
-      </c>
-      <c r="L7" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="I7" s="11">
+        <v>72.691100000000006</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.62749999999999995</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="0"/>
+        <v>8.6324185491758951E-3</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -788,15 +889,29 @@
         <v>2</v>
       </c>
       <c r="E8" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="7"/>
+        <v>0.3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="3">
+        <v>72.474400000000003</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.66590000000000005</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="0"/>
+        <v>9.1880719260870047E-3</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -818,9 +933,23 @@
         <v>7</v>
       </c>
       <c r="G9" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="L9" s="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="12">
+        <v>72.538799999999995</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0.53869999999999996</v>
+      </c>
+      <c r="K9" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4263704389926494E-3</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -836,46 +965,74 @@
         <v>2</v>
       </c>
       <c r="E10" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="3">
+        <v>72.537599999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.70789999999999997</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="0"/>
+        <v>9.7590766719604736E-3</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>30</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="7">
         <v>0.5</v>
       </c>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3">
-        <v>2</v>
-      </c>
-      <c r="E11" s="3">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="L11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="7">
+        <v>72.221999999999994</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0424801307080947E-2</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -884,15 +1041,31 @@
         <v>2</v>
       </c>
       <c r="E12" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L12" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="11">
+        <v>46.804000000000002</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.43819999999999998</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="0"/>
+        <v>9.3624476540466618E-3</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="16" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -916,7 +1089,21 @@
       <c r="G13" s="3">
         <v>0.3</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="H13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="3">
+        <v>46.622</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.56330000000000002</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.208227875252027E-2</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -940,7 +1127,21 @@
       <c r="G14" s="3">
         <v>0.5</v>
       </c>
-      <c r="L14" s="7"/>
+      <c r="H14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="12">
+        <v>46.6447</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0.42459999999999998</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" si="0"/>
+        <v>9.1028562730599612E-3</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="14"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -964,33 +1165,61 @@
       <c r="G15" s="3">
         <v>0.3</v>
       </c>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="s">
+      <c r="H15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="3">
+        <v>46.372</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.48249999999999998</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0404985767273355E-2</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="3">
-        <v>2</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7">
         <v>30</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="7">
         <v>0.5</v>
       </c>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="7">
+        <v>46.360700000000001</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0.50970000000000004</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0994225712726513E-2</v>
+      </c>
+      <c r="L16" s="10"/>
+      <c r="M16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -998,24 +1227,46 @@
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
       </c>
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
       <c r="F17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="3">
+        <v>91.107200000000006</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.33160000000000001</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="0"/>
+        <v>3.639668434547434E-3</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>20</v>
@@ -1023,48 +1274,79 @@
       <c r="D18" s="3">
         <v>2</v>
       </c>
+      <c r="E18" s="3">
+        <v>10</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
       </c>
+      <c r="E19" s="3">
+        <v>10</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3">
         <v>2</v>
       </c>
+      <c r="E20" s="3">
+        <v>10</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="3">
+        <v>72.653599999999997</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.64029999999999998</v>
+      </c>
+      <c r="K20" s="3">
+        <f>J20/I20</f>
+        <v>8.8130526223063957E-3</v>
+      </c>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -1072,22 +1354,28 @@
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="3">
         <v>2</v>
       </c>
+      <c r="E21" s="3">
+        <v>10</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
@@ -1095,66 +1383,91 @@
       <c r="D22" s="3">
         <v>2</v>
       </c>
+      <c r="E22" s="3">
+        <v>10</v>
+      </c>
       <c r="F22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
       </c>
+      <c r="E23" s="3">
+        <v>10</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3">
         <v>2</v>
       </c>
+      <c r="E24" s="3">
+        <v>10</v>
+      </c>
       <c r="F24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="G24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="7">
+        <v>2</v>
+      </c>
+      <c r="E25" s="7">
+        <v>10</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>12</v>
       </c>
@@ -1167,11 +1480,11 @@
       <c r="F26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L26" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
@@ -1184,9 +1497,9 @@
       <c r="F27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
@@ -1199,9 +1512,9 @@
       <c r="F28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>12</v>
       </c>
@@ -1214,9 +1527,9 @@
       <c r="F29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
@@ -1232,10 +1545,9 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="7"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1248,11 +1560,11 @@
       <c r="F31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
@@ -1263,11 +1575,11 @@
       <c r="F32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L32" s="7"/>
+      <c r="L32" s="6"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
@@ -1278,11 +1590,11 @@
       <c r="F33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="7"/>
+      <c r="L33" s="6"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>14</v>
@@ -1293,14 +1605,16 @@
       <c r="F34" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L34" s="7"/>
+      <c r="L34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="M2:M4"/>
+  <mergeCells count="6">
     <mergeCell ref="L2:L16"/>
     <mergeCell ref="L17:L25"/>
     <mergeCell ref="L26:L34"/>
+    <mergeCell ref="M2:M6"/>
+    <mergeCell ref="M7:M11"/>
+    <mergeCell ref="M12:M16"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1 E1:E1048576" xr:uid="{5BD20831-746F-FD45-BCE5-BD1EA2874D8B}">

</xml_diff>

<commit_message>
add SCP ensemble predictor
</commit_message>
<xml_diff>
--- a/report/experiment_plan.xlsx
+++ b/report/experiment_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengchen/GitHub/master_thesis/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BA4DA4-6553-1C4E-93D3-4F0A48450D44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96065DA6-0E7C-DB4E-94D7-9120BD5A5097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="3080" windowWidth="28800" windowHeight="15040" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
   </bookViews>
   <sheets>
     <sheet name="agg_50_trials" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="45">
   <si>
     <t>ACQ function</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>num_estimator = 10, special conformity score</t>
+  </si>
+  <si>
+    <t>num_estimator = 5</t>
+  </si>
+  <si>
+    <t>num_estimator = 10</t>
   </si>
 </sst>
 </file>
@@ -267,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -328,6 +334,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,10 +655,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BB70"/>
+  <dimension ref="A1:BB88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="98" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3149,7 +3158,7 @@
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D58" s="3">
         <v>2</v>
@@ -3169,29 +3178,29 @@
       <c r="I58" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="3">
-        <v>91.123999999999995</v>
-      </c>
-      <c r="K58" s="3">
-        <v>0.34739999999999999</v>
-      </c>
-      <c r="L58" s="3">
-        <f t="shared" ref="L57:L70" si="2">K58/J58</f>
-        <v>3.8123875159123831E-3</v>
+      <c r="J58" s="21">
+        <v>91.096599999999995</v>
+      </c>
+      <c r="K58" s="21">
+        <v>0.2132</v>
+      </c>
+      <c r="L58" s="21">
+        <f>K58/J58</f>
+        <v>2.3403727471716838E-3</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D59" s="3">
         <v>2</v>
@@ -3212,454 +3221,776 @@
         <v>17</v>
       </c>
       <c r="J59" s="3">
+        <v>91.123999999999995</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0.34739999999999999</v>
+      </c>
+      <c r="L59" s="3">
+        <f t="shared" ref="L59:L79" si="2">K59/J59</f>
+        <v>3.8123875159123831E-3</v>
+      </c>
+      <c r="N59" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="3">
+        <v>2</v>
+      </c>
+      <c r="E60" s="3">
+        <v>10</v>
+      </c>
+      <c r="F60" s="3">
+        <v>10</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" s="3">
         <v>91.0976</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K60" s="3">
         <v>0.2414</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L60" s="3">
         <f t="shared" si="2"/>
         <v>2.6499051566671351E-3</v>
       </c>
-      <c r="N59" s="3" t="s">
+      <c r="N60" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="3" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D60" s="3">
-        <v>2</v>
-      </c>
-      <c r="E60" s="3">
-        <v>10</v>
-      </c>
-      <c r="F60" s="3">
-        <v>10</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="C61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="3">
+        <v>2</v>
+      </c>
+      <c r="E61" s="3">
+        <v>10</v>
+      </c>
+      <c r="F61" s="3">
+        <v>10</v>
+      </c>
+      <c r="G61" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J60" s="3">
+      <c r="I61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" s="3">
         <v>91.018799999999999</v>
       </c>
-      <c r="K60" s="3">
+      <c r="K61" s="3">
         <v>0.26750000000000002</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L61" s="3">
         <f t="shared" si="2"/>
         <v>2.9389532711923253E-3</v>
       </c>
-      <c r="N60" s="3" t="s">
+      <c r="N61" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="3" t="s">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="3">
-        <v>2</v>
-      </c>
-      <c r="E61" s="3">
-        <v>10</v>
-      </c>
-      <c r="F61" s="3">
-        <v>10</v>
-      </c>
-      <c r="G61" s="3" t="s">
+      <c r="C62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="3">
+        <v>2</v>
+      </c>
+      <c r="E62" s="3">
+        <v>10</v>
+      </c>
+      <c r="F62" s="3">
+        <v>10</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J61" s="3">
+      <c r="I62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" s="3">
         <v>91.087599999999995</v>
       </c>
-      <c r="K61" s="3">
+      <c r="K62" s="3">
         <v>0.25269999999999998</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L62" s="3">
         <f t="shared" si="2"/>
         <v>2.7742524778345242E-3</v>
       </c>
-      <c r="N61" s="3" t="s">
+      <c r="N62" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="3" t="s">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D62" s="3">
-        <v>2</v>
-      </c>
-      <c r="E62" s="3">
-        <v>10</v>
-      </c>
-      <c r="F62" s="3">
-        <v>10</v>
-      </c>
-      <c r="G62" s="3" t="s">
+      <c r="C63" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="3">
+        <v>2</v>
+      </c>
+      <c r="E63" s="3">
+        <v>10</v>
+      </c>
+      <c r="F63" s="3">
+        <v>10</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" s="3">
+        <v>91.041200000000003</v>
+      </c>
+      <c r="K63" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="L63" s="3">
+        <f t="shared" si="2"/>
+        <v>2.8558498789559013E-3</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="3">
+        <v>2</v>
+      </c>
+      <c r="E64" s="3">
+        <v>10</v>
+      </c>
+      <c r="F64" s="3">
+        <v>10</v>
+      </c>
+      <c r="G64" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H64" s="3">
         <v>3</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J62" s="3">
+      <c r="I64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="3">
         <v>91.082999999999998</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K64" s="3">
         <v>0.26250000000000001</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L64" s="3">
         <f t="shared" si="2"/>
         <v>2.8819867593294032E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="3" t="s">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="3">
-        <v>2</v>
-      </c>
-      <c r="E63" s="3">
-        <v>10</v>
-      </c>
-      <c r="F63" s="3">
-        <v>10</v>
-      </c>
-      <c r="G63" s="3" t="s">
+      <c r="D65" s="3">
+        <v>2</v>
+      </c>
+      <c r="E65" s="3">
+        <v>10</v>
+      </c>
+      <c r="F65" s="3">
+        <v>10</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H63" s="3">
+      <c r="H65" s="3">
         <v>3</v>
       </c>
-      <c r="I63" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J63" s="8">
+      <c r="I65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" s="8">
         <v>91.191599999999994</v>
       </c>
-      <c r="K63" s="8">
+      <c r="K65" s="8">
         <v>0.26669999999999999</v>
       </c>
-      <c r="L63" s="8">
+      <c r="L65" s="8">
         <f t="shared" si="2"/>
         <v>2.9246114773729161E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="3" t="s">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D64" s="3">
-        <v>2</v>
-      </c>
-      <c r="E64" s="3">
-        <v>10</v>
-      </c>
-      <c r="F64" s="3">
-        <v>10</v>
-      </c>
-      <c r="G64" s="3" t="s">
+      <c r="D66" s="3">
+        <v>2</v>
+      </c>
+      <c r="E66" s="3">
+        <v>10</v>
+      </c>
+      <c r="F66" s="3">
+        <v>10</v>
+      </c>
+      <c r="G66" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H64" s="3">
+      <c r="H66" s="3">
         <v>3</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J64" s="3">
+      <c r="I66" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" s="3">
         <v>91.111800000000002</v>
       </c>
-      <c r="K64" s="3">
+      <c r="K66" s="3">
         <v>0.29730000000000001</v>
       </c>
-      <c r="L64" s="3">
+      <c r="L66" s="3">
         <f t="shared" si="2"/>
         <v>3.263024108842104E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" s="3" t="s">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="3">
-        <v>2</v>
-      </c>
-      <c r="E65" s="3">
-        <v>10</v>
-      </c>
-      <c r="F65" s="3">
-        <v>10</v>
-      </c>
-      <c r="G65" s="3" t="s">
+      <c r="D67" s="3">
+        <v>2</v>
+      </c>
+      <c r="E67" s="3">
+        <v>10</v>
+      </c>
+      <c r="F67" s="3">
+        <v>10</v>
+      </c>
+      <c r="G67" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H65" s="3">
+      <c r="H67" s="3">
         <v>3</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J65" s="3">
+      <c r="I67" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="3">
         <v>90.766800000000003</v>
       </c>
-      <c r="K65" s="3">
+      <c r="K67" s="3">
         <f>0.3409</f>
         <v>0.34089999999999998</v>
       </c>
-      <c r="L65" s="3">
+      <c r="L67" s="3">
         <f t="shared" si="2"/>
         <v>3.755778544577973E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+    <row r="68" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B68" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D68" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E66" s="5">
-        <v>10</v>
-      </c>
-      <c r="F66" s="5">
-        <v>10</v>
-      </c>
-      <c r="G66" s="5" t="s">
+      <c r="E68" s="5">
+        <v>10</v>
+      </c>
+      <c r="F68" s="5">
+        <v>10</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H66" s="5">
+      <c r="H68" s="5">
         <v>3</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" s="5">
+      <c r="I68" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="5">
         <v>91.0946</v>
       </c>
-      <c r="K66" s="5">
+      <c r="K68" s="5">
         <v>0.3251</v>
       </c>
-      <c r="L66" s="5">
+      <c r="L68" s="5">
         <f t="shared" si="2"/>
         <v>3.5688174710685376E-3</v>
       </c>
-      <c r="N66" s="11"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" s="3" t="s">
+      <c r="N68" s="11"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" s="3">
-        <v>2</v>
-      </c>
-      <c r="E67" s="3">
-        <v>10</v>
-      </c>
-      <c r="F67" s="3">
-        <v>10</v>
-      </c>
-      <c r="G67" s="3" t="s">
+      <c r="C69" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="3">
+        <v>2</v>
+      </c>
+      <c r="E69" s="3">
+        <v>10</v>
+      </c>
+      <c r="F69" s="3">
+        <v>10</v>
+      </c>
+      <c r="G69" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H69" s="3">
         <v>3</v>
       </c>
-      <c r="I67" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J67" s="3">
+      <c r="I69" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="3">
         <v>72.591899999999995</v>
       </c>
-      <c r="K67" s="3">
+      <c r="K69" s="3">
         <v>0.53990000000000005</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L69" s="3">
         <f t="shared" si="2"/>
         <v>7.4374689187085624E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B68" s="3" t="s">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="3">
-        <v>2</v>
-      </c>
-      <c r="E68" s="3">
-        <v>10</v>
-      </c>
-      <c r="F68" s="3">
-        <v>10</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="D70" s="3">
+        <v>2</v>
+      </c>
+      <c r="E70" s="3">
+        <v>10</v>
+      </c>
+      <c r="F70" s="3">
+        <v>10</v>
+      </c>
+      <c r="G70" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H68" s="3">
+      <c r="H70" s="3">
         <v>3</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J68" s="8">
+      <c r="I70" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="8">
         <v>72.8292</v>
       </c>
-      <c r="K68" s="8">
+      <c r="K70" s="8">
         <v>0.53700000000000003</v>
       </c>
-      <c r="L68" s="8">
+      <c r="L70" s="8">
         <f t="shared" si="2"/>
         <v>7.3734161572556068E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B69" s="3" t="s">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="3">
+        <v>2</v>
+      </c>
+      <c r="E71" s="3">
+        <v>10</v>
+      </c>
+      <c r="F71" s="3">
+        <v>10</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71" s="3">
+        <v>3</v>
+      </c>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="3">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3">
+        <v>10</v>
+      </c>
+      <c r="F72" s="3">
+        <v>10</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H72" s="3">
+        <v>3</v>
+      </c>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="3">
+        <v>10</v>
+      </c>
+      <c r="F73" s="3">
+        <v>10</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H73" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="3">
+        <v>10</v>
+      </c>
+      <c r="F74" s="3">
+        <v>10</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H74" s="3">
+        <v>3</v>
+      </c>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="3">
+        <v>2</v>
+      </c>
+      <c r="E75" s="3">
+        <v>10</v>
+      </c>
+      <c r="F75" s="3">
+        <v>10</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H75" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" s="3">
+        <v>2</v>
+      </c>
+      <c r="E76" s="3">
+        <v>10</v>
+      </c>
+      <c r="F76" s="3">
+        <v>10</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H76" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="8"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="3">
-        <v>2</v>
-      </c>
-      <c r="E69" s="3">
-        <v>10</v>
-      </c>
-      <c r="F69" s="3">
-        <v>10</v>
-      </c>
-      <c r="G69" s="3" t="s">
+      <c r="C78" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="3">
+        <v>2</v>
+      </c>
+      <c r="E78" s="3">
+        <v>10</v>
+      </c>
+      <c r="F78" s="3">
+        <v>10</v>
+      </c>
+      <c r="G78" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H69" s="3">
+      <c r="H78" s="3">
         <v>3</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J69" s="3">
+      <c r="I78" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" s="3">
         <v>46.6</v>
       </c>
-      <c r="K69" s="3">
+      <c r="K78" s="3">
         <v>0.39529999999999998</v>
       </c>
-      <c r="L69" s="3">
+      <c r="L78" s="3">
         <f t="shared" si="2"/>
         <v>8.4828326180257513E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B70" s="3" t="s">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="3">
-        <v>2</v>
-      </c>
-      <c r="E70" s="3">
-        <v>10</v>
-      </c>
-      <c r="F70" s="3">
-        <v>10</v>
-      </c>
-      <c r="G70" s="3" t="s">
+      <c r="D79" s="3">
+        <v>2</v>
+      </c>
+      <c r="E79" s="3">
+        <v>10</v>
+      </c>
+      <c r="F79" s="3">
+        <v>10</v>
+      </c>
+      <c r="G79" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H70" s="3">
+      <c r="H79" s="3">
         <v>3</v>
       </c>
-      <c r="I70" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J70" s="8">
+      <c r="I79" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J79" s="8">
         <v>46.79</v>
       </c>
-      <c r="K70" s="8">
+      <c r="K79" s="8">
         <v>0.43430000000000002</v>
       </c>
-      <c r="L70" s="8">
+      <c r="L79" s="8">
         <f t="shared" si="2"/>
         <v>9.281897841419107E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="3">
+        <v>10</v>
+      </c>
+      <c r="F80" s="3">
+        <v>10</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H80" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="3">
+        <v>10</v>
+      </c>
+      <c r="F81" s="3">
+        <v>10</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H81" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J87" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J88" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3674,29 +4005,29 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F37 F39:F43 F45:F1048576" xr:uid="{5BD20831-746F-FD45-BCE5-BD1EA2874D8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F37 F39:F43 F89:F1048576 F45:F86" xr:uid="{5BD20831-746F-FD45-BCE5-BD1EA2874D8B}">
       <formula1>"10, 30"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C37 C39:C43 C45:C1048576" xr:uid="{331C593D-BEE4-8448-91E2-4F45023D00DE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C37 C39:C43 C89:C1048576 C45:C86" xr:uid="{331C593D-BEE4-8448-91E2-4F45023D00DE}">
       <formula1>"ITS, PI, EI, UCB"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A43 A45:A1048576" xr:uid="{3725A888-F58A-6A43-B651-03A86BE31F1A}">
       <formula1>"mutation, random_sampling, dynamic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D37 D39:D43 D45:D1048576" xr:uid="{C9159AC4-0915-664B-9393-E3C5B0BCE85B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D37 D39:D43 D89:D1048576 D45:D86" xr:uid="{C9159AC4-0915-664B-9393-E3C5B0BCE85B}">
       <formula1>"2, 4, 6, NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E37 E39:E43 E45:E1048576" xr:uid="{646AD2B1-F937-6541-BDF5-B643AF2BD8CB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E37 E39:E43 E89:E1048576 E45:E86" xr:uid="{646AD2B1-F937-6541-BDF5-B643AF2BD8CB}">
       <formula1>"10,20,NA,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{DC0198F6-D5B8-7046-80E2-CEFE32AA7CAB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83:B1048576 B1:B81" xr:uid="{A6397971-01D4-F641-8567-4DAF687DF919}">
+      <formula1>"cifar10, cifar100, ImageNet16-120"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J87:J88 H89:H1048576 H1:H86" xr:uid="{DC0198F6-D5B8-7046-80E2-CEFE32AA7CAB}">
       <formula1>"NA, 0.3, 0.5, 3, 5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{E5123609-4FE5-E74A-B8B8-DF591FCA55AB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G89:G1048576 G1:G86" xr:uid="{E5123609-4FE5-E74A-B8B8-DF591FCA55AB}">
       <formula1>"Gaussian, SCP+ensembler, CVCP+quantile, SCP+quantile, CVCP+ensembler, BtCP"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A72 B74:B1048576 B1:B72" xr:uid="{A6397971-01D4-F641-8567-4DAF687DF919}">
-      <formula1>"cifar10, cifar100, ImageNet16-120"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update and add new plots
</commit_message>
<xml_diff>
--- a/report/experiment_plan.xlsx
+++ b/report/experiment_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chengchen/GitHub/master_thesis/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E0644E-B6B3-0640-87BB-03EC97540AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20500B86-DABD-2A48-9EC0-84F307ACC251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F6D8400F-B912-A94E-8399-434B778D62B2}"/>
   </bookViews>
   <sheets>
     <sheet name="agg_50_trials" sheetId="1" r:id="rId1"/>
@@ -374,14 +374,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +702,8 @@
   </sheetPr>
   <dimension ref="A1:BA98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:XFD88"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,41 +769,41 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:14" s="28" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="28">
+        <v>2</v>
+      </c>
+      <c r="E2" s="28">
+        <v>10</v>
+      </c>
+      <c r="F2" s="28">
+        <v>10</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="I2" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="29">
         <v>91.148399999999995</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="28">
         <v>0.28520000000000001</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="28">
         <f t="shared" ref="L2:L33" si="0">K2/J2</f>
         <v>3.1289633169644233E-3</v>
       </c>
@@ -896,41 +896,41 @@
       <c r="M4" s="22"/>
       <c r="N4" s="25"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="28">
+        <v>2</v>
+      </c>
+      <c r="E5" s="28">
+        <v>10</v>
+      </c>
+      <c r="F5" s="28">
+        <v>10</v>
+      </c>
+      <c r="G5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="28">
         <v>0.5</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="7">
+      <c r="I5" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="30">
         <v>91.130399999999995</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="30">
         <v>0.23200000000000001</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="30">
         <f t="shared" si="0"/>
         <v>2.5458024983979004E-3</v>
       </c>
@@ -3772,45 +3772,44 @@
         <v>3.755778544577973E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:14" s="28" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" s="28" t="s">
+    <row r="72" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="28" t="s">
+      <c r="C72" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="28">
-        <v>2</v>
-      </c>
-      <c r="E72" s="28">
+      <c r="D72" s="3">
+        <v>2</v>
+      </c>
+      <c r="E72" s="3">
         <v>20</v>
       </c>
-      <c r="F72" s="28">
-        <v>10</v>
-      </c>
-      <c r="G72" s="28" t="s">
+      <c r="F72" s="3">
+        <v>10</v>
+      </c>
+      <c r="G72" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H72" s="28">
+      <c r="H72" s="3">
         <v>3</v>
       </c>
-      <c r="I72" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="J72" s="29">
+      <c r="I72" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" s="8">
         <v>91.213399999999993</v>
       </c>
-      <c r="K72" s="29">
+      <c r="K72" s="8">
         <v>0.23419999999999999</v>
       </c>
-      <c r="L72" s="29">
+      <c r="L72" s="8">
         <f>K72/J72</f>
         <v>2.567605198359013E-3</v>
       </c>
-      <c r="N72" s="30"/>
     </row>
     <row r="73" spans="1:14" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
@@ -3930,45 +3929,44 @@
         <v>7.3734161572556068E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" s="28" t="s">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="28" t="s">
+      <c r="C76" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="28">
-        <v>2</v>
-      </c>
-      <c r="E76" s="28">
+      <c r="D76" s="3">
+        <v>2</v>
+      </c>
+      <c r="E76" s="3">
         <v>20</v>
       </c>
-      <c r="F76" s="28">
-        <v>10</v>
-      </c>
-      <c r="G76" s="28" t="s">
+      <c r="F76" s="3">
+        <v>10</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H76" s="28">
+      <c r="H76" s="3">
         <v>3</v>
       </c>
-      <c r="I76" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="J76" s="29">
+      <c r="I76" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" s="8">
         <v>72.848799999999997</v>
       </c>
-      <c r="K76" s="29">
+      <c r="K76" s="8">
         <v>0.4602</v>
       </c>
-      <c r="L76" s="29">
+      <c r="L76" s="8">
         <f t="shared" si="2"/>
         <v>6.3171939688780052E-3</v>
       </c>
-      <c r="N76" s="30"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
@@ -4415,45 +4413,44 @@
         <v>9.281897841419107E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B88" s="28" t="s">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C88" s="28" t="s">
+      <c r="C88" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="28">
-        <v>2</v>
-      </c>
-      <c r="E88" s="28">
+      <c r="D88" s="3">
+        <v>2</v>
+      </c>
+      <c r="E88" s="3">
         <v>20</v>
       </c>
-      <c r="F88" s="28">
-        <v>10</v>
-      </c>
-      <c r="G88" s="28" t="s">
+      <c r="F88" s="3">
+        <v>10</v>
+      </c>
+      <c r="G88" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H88" s="28">
+      <c r="H88" s="3">
         <v>3</v>
       </c>
-      <c r="I88" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="J88" s="28">
+      <c r="I88" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J88" s="3">
         <v>46.66</v>
       </c>
-      <c r="K88" s="28">
+      <c r="K88" s="3">
         <v>0.46360000000000001</v>
       </c>
-      <c r="L88" s="28">
+      <c r="L88" s="3">
         <f t="shared" ref="L88:L95" si="4">K88/J88</f>
         <v>9.9357051007286767E-3</v>
       </c>
-      <c r="N88" s="30"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
@@ -4574,7 +4571,7 @@
       </c>
       <c r="N91" s="11"/>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>